<commit_message>
Updated to match LS name
</commit_message>
<xml_diff>
--- a/hyperlinker/app/referencesheets/MLS Intake Paralegal Splitter.xlsx
+++ b/hyperlinker/app/referencesheets/MLS Intake Paralegal Splitter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shrene\Python\GitPython\hyperlinker\app\referencesheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B97902A8-6A21-4A6E-9B13-F5C29D08A289}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB23CB85-9239-468B-9F1F-092DF84D54B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{4180EAC3-DA45-4891-B57C-B18591B224AC}"/>
   </bookViews>
@@ -177,9 +177,6 @@
     <t>Villanueva, Anthony</t>
   </si>
   <si>
-    <t>Trinidad, Ayla</t>
-  </si>
-  <si>
     <t>Avila, Giselle L</t>
   </si>
   <si>
@@ -211,6 +208,9 @@
   </si>
   <si>
     <t>Harris, Tycel M</t>
+  </si>
+  <si>
+    <t>Trinidad, Ayla A</t>
   </si>
 </sst>
 </file>
@@ -686,7 +686,7 @@
         <v>34</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>19</v>
@@ -709,7 +709,7 @@
         <v>35</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>18</v>
@@ -735,7 +735,7 @@
         <v>10</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -746,7 +746,7 @@
         <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D6" t="s">
         <v>30</v>
@@ -766,7 +766,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
@@ -781,12 +781,12 @@
         <v>7</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>23</v>
@@ -803,16 +803,16 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>49</v>
@@ -823,10 +823,10 @@
         <v>27</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>